<commit_message>
Update JS Exam materials
</commit_message>
<xml_diff>
--- a/Modul-1/JavaScript-Fundamentals/Materials/MatrixExample.xlsx
+++ b/Modul-1/JavaScript-Fundamentals/Materials/MatrixExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikito\Documents\Telerik Academy Master\Owolp\Modul-1\JavaScript-Fundamentals\Exam-Preparation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zikito\Documents\Telerik Academy Master\Owolp\Modul-1\JavaScript-Fundamentals\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Indexed Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,9 +25,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>6x7</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>3,0</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>5,0</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>5,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>5,2</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>4,5</t>
   </si>
 </sst>
 </file>
@@ -65,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,14 +182,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +528,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,4 +725,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="7" width="9.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>